<commit_message>
check Mr. Ahgili work
</commit_message>
<xml_diff>
--- a/app/src/docs/ToDo.xlsx
+++ b/app/src/docs/ToDo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="235">
   <si>
     <t>ActivityLogin</t>
   </si>
@@ -832,6 +832,30 @@
   </si>
   <si>
     <t>Force close: getResult (if webservice is executed)</t>
+  </si>
+  <si>
+    <t>ViewHolder -&gt; initial() -&gt;this.options.setOnClickListener : 
+line 135</t>
+  </si>
+  <si>
+    <t>update list after deleting one post</t>
+  </si>
+  <si>
+    <t>ActivityNewBusiness_step1</t>
+  </si>
+  <si>
+    <t>put progress dialog for chaging categroy spinner and executing
+GetSubcategories</t>
+  </si>
+  <si>
+    <t>pass wrong business.id to the ActivityNewBusienss_step2.
+check ActivityNewBusienss_step2 line 166 to see worng id.</t>
+  </si>
+  <si>
+    <t>If user have 0 friend or review or followed business:
+Don't go to the related pages
+If business have 0 follower or review:
+Don't go to the related pages</t>
   </si>
 </sst>
 </file>
@@ -1240,10 +1264,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F175"/>
+  <dimension ref="A1:F182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A165" workbookViewId="0">
-      <selection activeCell="B172" sqref="B172"/>
+    <sheetView tabSelected="1" topLeftCell="A173" workbookViewId="0">
+      <selection activeCell="A182" sqref="A182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2564,8 +2588,52 @@
         <v>228</v>
       </c>
     </row>
+    <row r="177" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="10">
+        <v>42056</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A178" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A179" s="19"/>
+      <c r="B179" s="1" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A180" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A181" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A182" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A178:A179"/>
     <mergeCell ref="A135:A138"/>
     <mergeCell ref="A146:A148"/>
     <mergeCell ref="A158:A159"/>

</xml_diff>

<commit_message>
add some tasks ToDo.xlsx
</commit_message>
<xml_diff>
--- a/app/src/docs/ToDo.xlsx
+++ b/app/src/docs/ToDo.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="260">
   <si>
     <t>ActivityLogin</t>
   </si>
@@ -898,6 +898,47 @@
   </si>
   <si>
     <t>Display result in listview, getResult: line 195</t>
+  </si>
+  <si>
+    <t>Implement RequestConfirmation in View layout</t>
+  </si>
+  <si>
+    <t>It is the second time I mention it!</t>
+  </si>
+  <si>
+    <t>Add sent comment to listview</t>
+  </si>
+  <si>
+    <t>Clear comment edittext after successfully executing SendComment webservice</t>
+  </si>
+  <si>
+    <t>update post comment number in adapter after successfully executing
+ SendComment webservice</t>
+  </si>
+  <si>
+    <t>In unseen.xlsx file for " Comment on post" you said:
+«کامنت قرار میگیرد اما تعداد کامنت ها به درستی نمایش داده نمیشوند»</t>
+  </si>
+  <si>
+    <t>what did you mean?</t>
+  </si>
+  <si>
+    <t>Where did you call GetAllCommentNotifications?</t>
+  </si>
+  <si>
+    <t>Loadmore data for business' post when business has no more posts</t>
+  </si>
+  <si>
+    <t>How do you rate a business?!!!</t>
+  </si>
+  <si>
+    <t>there is no option in View layout</t>
+  </si>
+  <si>
+    <t>ForceClose after successfully executing Like webservice</t>
+  </si>
+  <si>
+    <t>Implement Unlike</t>
   </si>
 </sst>
 </file>
@@ -977,7 +1018,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1022,6 +1063,12 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1327,10 +1374,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F191"/>
+  <dimension ref="A1:F202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="A192" sqref="A192"/>
+    <sheetView tabSelected="1" topLeftCell="A189" workbookViewId="0">
+      <selection activeCell="A197" sqref="A197:XFD197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2754,10 +2801,89 @@
         <v>246</v>
       </c>
     </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="12" t="s">
+        <v>247</v>
+      </c>
+      <c r="B192" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A193" s="24" t="s">
+        <v>226</v>
+      </c>
+      <c r="B193" s="18" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A194" s="24"/>
+      <c r="B194" s="18" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A195" s="24"/>
+      <c r="B195" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="B196" s="18" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A197" s="12" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A198" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="B198" s="18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B199" s="28" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A200" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="B200" s="18" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A201" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B201" s="18" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" s="18" t="s">
+        <v>259</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="A185:A186"/>
     <mergeCell ref="A190:A191"/>
+    <mergeCell ref="A193:A195"/>
     <mergeCell ref="A178:A179"/>
     <mergeCell ref="A135:A138"/>
     <mergeCell ref="A146:A148"/>

</xml_diff>